<commit_message>
changed led IC and schematic
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B82016E-25B2-49ED-9F80-6453CE99CCDD}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3323067D-CC6F-4F5F-8CF2-4A7F8ECC8AB6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="1104" windowWidth="17244" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,7 +497,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D7" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
First hardware pwm test
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3323067D-CC6F-4F5F-8CF2-4A7F8ECC8AB6}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8BB351B-A6B3-402F-802D-6BCA2721DA7E}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="1104" windowWidth="17244" windowHeight="8868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Datum</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Worked on schematic for led, tested led, read datasheet led and led-driver</t>
+  </si>
+  <si>
+    <t>Worked on schematic for led with new chip, solderd current driver for led for testing, created fresh raspberry pi image.</t>
   </si>
 </sst>
 </file>
@@ -393,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,9 +507,18 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="2">
+        <v>44809</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>

</xml_diff>

<commit_message>
added schematics, updated log, added conversation
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8BB351B-A6B3-402F-802D-6BCA2721DA7E}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2FAD91A-FA6C-4570-8885-45D411A56B2D}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
     <t>Worked on schematic for led, tested led, read datasheet led and led-driver</t>
   </si>
   <si>
-    <t>Worked on schematic for led with new chip, solderd current driver for led for testing, created fresh raspberry pi image.</t>
+    <t>Worked on schematic for led with new chip, solderd cn5711 driver for led for testing, back-upped old and created fresh raspberry pi image. Wrote hardware pwm code python for cn5711 chip (ldo6ajsa)</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,15 +514,19 @@
         <v>0.375</v>
       </c>
       <c r="D8" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="2">
+        <v>44810</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
started design on PMS added components and values
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2FAD91A-FA6C-4570-8885-45D411A56B2D}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44366CBC-F270-440B-B0CE-AB3BF7BA9AEB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Datum</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Worked on schematic for led with new chip, solderd cn5711 driver for led for testing, back-upped old and created fresh raspberry pi image. Wrote hardware pwm code python for cn5711 chip (ldo6ajsa)</t>
+  </si>
+  <si>
+    <t>worked on schematic, helped students via meeting, started power management system design, tried to test stepper motor driver</t>
   </si>
 </sst>
 </file>
@@ -396,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,11 +530,20 @@
       <c r="C9" s="3">
         <v>0.36458333333333331</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="3">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="2">
+        <v>44811</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added drv8838 in design as option for focussing motors
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD0DF19C-19E2-4881-9EB0-DEC53F50DAA9}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E86E546-7178-4BFE-B927-61024787538F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Worked on schematic, started heating and cooling design, updated a lot of designs and talked with jeroen.</t>
+  </si>
+  <si>
+    <t>found a H-bridge for peltier module and integrated it in the schematic, worked on the documentation (choices etc)</t>
   </si>
 </sst>
 </file>
@@ -579,6 +582,9 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D12" s="1"/>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>

</xml_diff>

<commit_message>
documentation and schematic improvements
documentation updated, design choices update on led driver
added esd protection options diodes and ic for i2c esd protection
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E86E546-7178-4BFE-B927-61024787538F}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F39E1EB3-2771-4CFC-B071-79AA22664E3D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>found a H-bridge for peltier module and integrated it in the schematic, worked on the documentation (choices etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added labels to trello (absolutely necessary) </t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,15 +584,24 @@
       <c r="C12" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="3">
+        <v>0.625</v>
+      </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="2">
+        <v>44816</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.36458333333333331</v>
+      </c>
       <c r="D13" s="1"/>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>

</xml_diff>

<commit_message>
Updated H-bridge schematic + Use case diagram
 included decoupling capacitors
Started working on use case diagram
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F31086F-6B6E-4BE4-B218-E65AF51DE96C}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37F600B1-B9CC-416F-BD4F-A97786CF5D05}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20064" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>added labels to trello, added ESD circuit to i2c, tried to get tmc2208 to work:  no succes. Helped students with their projects/questions and gathered emergency materials from Jelle. Created 5V PSU for breadboard</t>
+  </si>
+  <si>
+    <t>talked with Johan Korten about my diagrams and further actions. Prepared for meeting (drew global setting of HCL), meeting with HCL and requested. Called with Jelle about lab materials and prepared a plan to call with jelle and jeroen in the (near) future.</t>
   </si>
 </sst>
 </file>
@@ -411,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,9 +609,16 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="2">
+        <v>44817</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.375</v>
+      </c>
       <c r="D14" s="1"/>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>

</xml_diff>

<commit_message>
assigent footprints to all current components
I chose 1206smd handsolderable for caps and resistors and inductors, may need to be revised
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37F600B1-B9CC-416F-BD4F-A97786CF5D05}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A87BE09-A714-4179-AB6C-998372B6B717}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="20064" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>added labels to trello, added ESD circuit to i2c, tried to get tmc2208 to work:  no succes. Helped students with their projects/questions and gathered emergency materials from Jelle. Created 5V PSU for breadboard</t>
   </si>
   <si>
-    <t>talked with Johan Korten about my diagrams and further actions. Prepared for meeting (drew global setting of HCL), meeting with HCL and requested. Called with Jelle about lab materials and prepared a plan to call with jelle and jeroen in the (near) future.</t>
+    <t>talked with Johan Korten about my diagrams and further actions. Prepared for meeting (drew global setting of HCL), meeting with HCL and requested. Called with Jelle about lab materials and prepared a plan to call with jelle and jeroen in the (near) future. Figured out how to add custom footprints to kicadV6</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
ended log of the day
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A87BE09-A714-4179-AB6C-998372B6B717}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92AB4918-EEC5-41A2-BF34-CDDD4ECC157F}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="20064" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>added labels to trello, added ESD circuit to i2c, tried to get tmc2208 to work:  no succes. Helped students with their projects/questions and gathered emergency materials from Jelle. Created 5V PSU for breadboard</t>
   </si>
   <si>
-    <t>talked with Johan Korten about my diagrams and further actions. Prepared for meeting (drew global setting of HCL), meeting with HCL and requested. Called with Jelle about lab materials and prepared a plan to call with jelle and jeroen in the (near) future. Figured out how to add custom footprints to kicadV6</t>
+    <t>talked with Johan Korten about my diagrams and further actions. Prepared for meeting (drew global setting of HCL), meeting with HCL and requested. Called with Jelle about lab materials and prepared a plan to call with jelle and jeroen in the (near) future. Figured out how to add custom footprints to kicadV6. Fixed the snapeda desktop edition and fixed the Mouser SamacSys part / footprint downloaders integration with kicadv6. Added footprints to all components and started pcb template</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,9 @@
       <c r="C14" s="3">
         <v>0.375</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="3">
+        <v>0.69791666666666663</v>
+      </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
updated footprints for pcb design
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92AB4918-EEC5-41A2-BF34-CDDD4ECC157F}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF77515-96D4-443E-8DC9-584088518A79}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="20064" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,8 +623,12 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="2">
+        <v>44818</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.38541666666666669</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added 2 GPIO power pins (high loads)
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AF77515-96D4-443E-8DC9-584088518A79}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EFC11FD-2B34-46A2-A17D-651E8203FADF}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>talked with Johan Korten about my diagrams and further actions. Prepared for meeting (drew global setting of HCL), meeting with HCL and requested. Called with Jelle about lab materials and prepared a plan to call with jelle and jeroen in the (near) future. Figured out how to add custom footprints to kicadV6. Fixed the snapeda desktop edition and fixed the Mouser SamacSys part / footprint downloaders integration with kicadv6. Added footprints to all components and started pcb template</t>
+  </si>
+  <si>
+    <t>worked on schematic, added rpi connector and tested A4988 stepper motor driver</t>
+  </si>
+  <si>
+    <t>New approach tested (shorter work time, more productivity?), Improved schematic, included data from Jeroen's stepper setup</t>
   </si>
 </sst>
 </file>
@@ -414,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,12 +635,26 @@
       <c r="C15" s="3">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="2">
+        <v>44819</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>

</xml_diff>

<commit_message>
updated some connectors to jst xh2.54
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{312E1061-F6F0-416D-A39F-004A696FF624}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39820DB7-79D6-44FD-AF12-BD49A740C5D0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -49,21 +49,6 @@
     <t>Bezigheden</t>
   </si>
   <si>
-    <t>Intro gesprek met Jeroen</t>
-  </si>
-  <si>
-    <t>kickoff +  gewerkt aan POA</t>
-  </si>
-  <si>
-    <t>gewerkt POA, gesprek met jeroen product functionaliteit, uitwerkingen</t>
-  </si>
-  <si>
-    <t>gewerkt aan globaal ontwerp, kesselring overweging, gesprek met jeroen globaal ontwerp.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gewerkt aan pro's en con's lijst opzetje. State diagram gemaakt. Systeem architectuur aangepast na gesprek met Jeroen. </t>
-  </si>
-  <si>
     <t>Worked on schematic for led, tested led, read datasheet led and led-driver</t>
   </si>
   <si>
@@ -97,7 +82,25 @@
     <t>X</t>
   </si>
   <si>
-    <t>Finished schematic (ready for big review), installed piqt in pycharm, talked with S3 project groups about their proces</t>
+    <t>Finished schematic (ready for big review), installed piqt in pycharm, talked with S3 project groups about their proces. Made a knob in pyqt that controls RPI hardware PWM pin.</t>
+  </si>
+  <si>
+    <t>Intro conversation with Jeroen Veen</t>
+  </si>
+  <si>
+    <t>kickoff +  worked on POA</t>
+  </si>
+  <si>
+    <t>Worked on POA, conversation with jeroen about product functionality, details</t>
+  </si>
+  <si>
+    <t>Worked on global design, kesselring methode, conversation jeroen about global design.</t>
+  </si>
+  <si>
+    <t>Pros and cons list created. State diagram created. Systeem architectuur enhanced after conversation with jeroen</t>
+  </si>
+  <si>
+    <t>Tidied up component boxes and sorted components for extra efficiency and component ESD safety. Attended workshop (20 min) enh connectors schematic</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,7 +466,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -477,7 +480,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -491,7 +494,7 @@
         <v>0.625</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -505,7 +508,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -519,7 +522,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -533,7 +536,7 @@
         <v>0.6875</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -547,7 +550,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -561,7 +564,7 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -575,7 +578,7 @@
         <v>0.6875</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -589,7 +592,7 @@
         <v>0.6875</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -603,7 +606,7 @@
         <v>0.625</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -617,7 +620,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -631,7 +634,7 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
@@ -645,7 +648,7 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -659,7 +662,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -667,13 +670,13 @@
         <v>44820</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -683,15 +686,24 @@
       <c r="C18" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="3">
+        <v>0.625</v>
+      </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="B19" s="2">
+        <v>44824</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D19" s="1"/>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>

</xml_diff>

<commit_message>
cleanup and changed some names to Rastaban
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CAF2707-CA71-49C1-B58C-4F78576F650F}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5EF2833-E196-4214-94D5-FA7066D00DA7}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <t>Tidied up component boxes and sorted components for extra efficiency and component ESD safety. Attended workshop (20 min),  enh connectors schematic. Read trough S6 project's code.</t>
   </si>
   <si>
-    <t>Set-up raspberry pi remote connect (SSH) with VSC and github. Tested LED software remotely on pi. Tried to get QTPY knob working via ssh</t>
+    <t>Set-up raspberry pi remote connect (SSH) with VSC and github. Tested LED software remotely on pi. Got QTPY knob working via ssh (PYQT5)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Heavily improved symbol text placements
all texts are now readable
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{592D326B-A6AA-45A0-A2DE-1AD548393F47}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B7E2EA2-5F5C-4CC2-961E-358DD083FC25}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Set-up raspberry pi remote connect (SSH) with VSC and github. Tested LED software remotely on pi. Got QTPY knob working via ssh (PYQT5) conversation with Jeroen about pcb, schematic, software development and testing</t>
+  </si>
+  <si>
+    <t>Fixed schematic V1.0 by using all the notes that jeroen has created on that version. Found new parts and attended interview at the fablab.</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,15 +720,24 @@
       <c r="C20" s="3">
         <v>0.40625</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="3">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="E20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>

</xml_diff>

<commit_message>
new i2c protection circuit
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B7E2EA2-5F5C-4CC2-961E-358DD083FC25}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C58EB339-C18B-41C4-9416-1667384937C4}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Fixed schematic V1.0 by using all the notes that jeroen has created on that version. Found new parts and attended interview at the fablab.</t>
+  </si>
+  <si>
+    <t>gained more info on pyqt slots and signals. Bought a book on pyqt5, read it for a part and practised design skills</t>
   </si>
 </sst>
 </file>
@@ -435,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,8 +744,15 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="C22" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>

</xml_diff>

<commit_message>
Added new connectors for stepper motors Phoenix PTSM
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crtak\HAN\Jeroen Veen - Effluent\07 Studentprojects\Casper Tak\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="11_AD4DB114E441178AC67DF4A82ED4FA90693EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C58EB339-C18B-41C4-9416-1667384937C4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>gained more info on pyqt slots and signals. Bought a book on pyqt5, read it for a part and practised design skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read in the pyqt book, tried sliders and knobs and ticks etc. </t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +734,9 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
+      <c r="B21" s="2">
+        <v>44826</v>
+      </c>
       <c r="C21" s="3">
         <v>0.41666666666666669</v>
       </c>
@@ -743,7 +748,9 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
+      <c r="B22" s="2">
+        <v>44827</v>
+      </c>
       <c r="C22" s="3">
         <v>0.47916666666666669</v>
       </c>
@@ -755,9 +762,16 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="B23" s="2">
+        <v>44830</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>

</xml_diff>

<commit_message>
added connector footprint to schematic
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crtak\HAN\Jeroen Veen - Effluent\07 Studentprojects\Casper Tak\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{544CBAF0-EAC2-480A-B4E5-C8591E0117F3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
     <t>gained more info on pyqt slots and signals. Bought a book on pyqt5, read it for a part and practised design skills</t>
   </si>
   <si>
-    <t xml:space="preserve">Read in the pyqt book, tried sliders and knobs and ticks etc. </t>
+    <t>Read in the pyqt book, tried sliders and knobs and ticks etc. added phoenix ptsm connectors to schematic</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Created concept for GUI python control.
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{544CBAF0-EAC2-480A-B4E5-C8591E0117F3}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A9AFCDA-A426-49E2-9431-4B72031A26F9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <t>gained more info on pyqt slots and signals. Bought a book on pyqt5, read it for a part and practised design skills</t>
   </si>
   <si>
-    <t>Read in the pyqt book, tried sliders and knobs and ticks etc. added phoenix ptsm connectors to schematic</t>
+    <t>Read in the pyqt book, tried sliders and knobs and ticks etc. added phoenix ptsm connectors to schematic. Created GUI concept in draw.io for a better understanding of what to create</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixed eeprom esd protection
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A9AFCDA-A426-49E2-9431-4B72031A26F9}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB792F7-2F9E-4717-B1F3-50768CEA44D1}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Datum</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Read in the pyqt book, tried sliders and knobs and ticks etc. added phoenix ptsm connectors to schematic. Created GUI concept in draw.io for a better understanding of what to create</t>
+  </si>
+  <si>
+    <t>Python code for tmc2209 writen.</t>
   </si>
 </sst>
 </file>
@@ -441,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,15 +771,24 @@
       <c r="C23" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="3">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="B24" s="2">
+        <v>44831</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D24" s="1"/>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>

</xml_diff>

<commit_message>
added new libarries and jlcpcb part plugin
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9976F5F-92BB-4C59-8321-B82AFEBE1640}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67666728-96A0-4C16-A3A3-314681A50192}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>worked on GUI. Read the pyqt5 book. Got a working A4498 stepper motor setup. Read on OOP with python.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">python stepper motor working, made test report, talked with johan brussen about schematic. Cleanup up kicad (libraries where bad) </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>watched and learned from videos on python OOP. Tried to create main window, but required data from jeroen. Expirimented with kicad export functionality.</t>
+  </si>
+  <si>
+    <t>C3339</t>
+  </si>
+  <si>
+    <t>C160404</t>
+  </si>
+  <si>
+    <t>C513765</t>
+  </si>
+  <si>
+    <t>C525005</t>
+  </si>
+  <si>
+    <t>C2918513</t>
   </si>
 </sst>
 </file>
@@ -447,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,19 +834,44 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="B26" s="2">
+        <v>44833</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="B27" s="2">
+        <v>44834</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="2">
+        <v>44837</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.40625</v>
+      </c>
       <c r="D28" s="1"/>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
@@ -1092,32 +1141,44 @@
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
+      <c r="D82" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
+      <c r="D83" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
+      <c r="D84" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
+      <c r="D85" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="1"/>

</xml_diff>

<commit_message>
python book, kicad plugin
Added python book
installed kicad plugin that saves hours of time finding LCSC parts for pcb assembly (kicad jlcpcb tools)
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67666728-96A0-4C16-A3A3-314681A50192}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8222B588-F5CB-45E3-9AD0-64F3722CE565}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Datum</t>
   </si>
@@ -128,21 +128,6 @@
   </si>
   <si>
     <t>watched and learned from videos on python OOP. Tried to create main window, but required data from jeroen. Expirimented with kicad export functionality.</t>
-  </si>
-  <si>
-    <t>C3339</t>
-  </si>
-  <si>
-    <t>C160404</t>
-  </si>
-  <si>
-    <t>C513765</t>
-  </si>
-  <si>
-    <t>C525005</t>
-  </si>
-  <si>
-    <t>C2918513</t>
   </si>
 </sst>
 </file>
@@ -471,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82:D87"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,14 +853,20 @@
       <c r="C28" s="3">
         <v>0.40625</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="2">
+        <v>44838</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.42708333333333331</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
@@ -1141,44 +1132,32 @@
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-      <c r="D82" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="D82" s="1"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-      <c r="D83" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="D83" s="1"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-      <c r="D84" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="D84" s="1"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="D85" s="1"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D86" s="1"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-      <c r="D87" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="D87" s="1"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="1"/>

</xml_diff>

<commit_message>
removed warnings in PCB new by fixing footprints
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8222B588-F5CB-45E3-9AD0-64F3722CE565}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE136BA0-467A-447F-B6C2-E687C338D4A5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29460" yWindow="720" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Datum</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>watched and learned from videos on python OOP. Tried to create main window, but required data from jeroen. Expirimented with kicad export functionality.</t>
+  </si>
+  <si>
+    <t>started learning python with new book, worked on PCB footprints and lcsc part list</t>
+  </si>
+  <si>
+    <t>Worked on PCB footprints.</t>
   </si>
 </sst>
 </file>
@@ -456,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,12 +873,24 @@
       <c r="C29" s="3">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="2">
+        <v>44839</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D30" s="1"/>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>

</xml_diff>

<commit_message>
All files created with Jan
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE136BA0-467A-447F-B6C2-E687C338D4A5}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{825EA7A6-C3E2-4F7E-9A32-A34AEDB5274C}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="720" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Datum</t>
   </si>
@@ -133,7 +133,16 @@
     <t>started learning python with new book, worked on PCB footprints and lcsc part list</t>
   </si>
   <si>
-    <t>Worked on PCB footprints.</t>
+    <t>Worked on PCB footprints and added 3d models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x </t>
+  </si>
+  <si>
+    <t>Worked on pcb layout, improved pcb workflow skills (to prevent wasting time)</t>
+  </si>
+  <si>
+    <t>Worked on software architecture, with the help of Jan.</t>
   </si>
 </sst>
 </file>
@@ -462,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,97 +896,124 @@
       <c r="C30" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="3">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E30" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="B31" s="2">
+        <v>44840</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="B32" s="2">
+        <v>44841</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>44844</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.3888888888888889</v>
+      </c>
       <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>

</xml_diff>

<commit_message>
general layout created pcb
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{825EA7A6-C3E2-4F7E-9A32-A34AEDB5274C}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B7057DD-7813-4702-A14E-8FA7B0C1A5B1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,7 +142,7 @@
     <t>Worked on pcb layout, improved pcb workflow skills (to prevent wasting time)</t>
   </si>
   <si>
-    <t>Worked on software architecture, with the help of Jan.</t>
+    <t>Worked on software architecture, with the help of Jan. Created new PCB layout (grouped components together)</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +938,9 @@
       <c r="C33" s="3">
         <v>0.3888888888888889</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E33" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
changed mosfets to cheaper and smaller alternatives
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82F4009E-7A4B-48E0-98D7-CA913E934EF9}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F2F5CF5-1913-419A-A608-C9EF71123080}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20250" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Datum</t>
   </si>
@@ -145,7 +145,10 @@
     <t>Worked on software architecture, with the help of Jan. Created new PCB layout (grouped components together)</t>
   </si>
   <si>
-    <t>Worked on pcb layout</t>
+    <t xml:space="preserve">Worked on pcb layout. Long meeting with jeroen and rudie and johan k. </t>
+  </si>
+  <si>
+    <t>explained why to choose PHOENIX instead of JST. Added connectors to pcb. Searched for better components</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,15 +958,24 @@
       <c r="C34" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="3">
+        <v>0.65625</v>
+      </c>
       <c r="E34" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="B35" s="2">
+        <v>44846</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.3888888888888889</v>
+      </c>
       <c r="D35" s="1"/>
+      <c r="E35" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>

</xml_diff>

<commit_message>
started routing biger traces
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09225167-8FBF-4290-ACE1-B9222DF90017}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A40499F-4A98-400F-9420-420DE26E44A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,7 +1006,9 @@
       <c r="C37" s="3">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="3">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E37" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
started creating bigger traces for power
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A40499F-4A98-400F-9420-420DE26E44A6}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{835E88B9-5B0C-4A83-AAA3-FDAEFDDDDDB3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Datum</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Studied using udemy python course, started and finished routing PCB.  (I was ill this day)</t>
+  </si>
+  <si>
+    <t>Sick</t>
+  </si>
+  <si>
+    <t>worked on pcb, talked with johan b about pcb, talked with johan k on software design</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,6 +206,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,23 +1023,54 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="B38" s="2">
+        <v>44852</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="B39" s="2">
+        <v>44853</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
+      <c r="B40" s="2">
+        <v>44854</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="B41" s="2">
+        <v>44855</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.49305555555555558</v>
+      </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Worked on presentation and wiring pcb
ERC: 0 error, 30 warnings
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{835E88B9-5B0C-4A83-AAA3-FDAEFDDDDDB3}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7830F22F-653E-468A-A38B-E34FD6CFED59}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>worked on pcb, talked with johan b about pcb, talked with johan k on software design</t>
+  </si>
+  <si>
+    <t>worked on pcb trace thickness</t>
+  </si>
+  <si>
+    <t>worked on PPT presentation for Thursday and enlarged pcb traces (for power)</t>
   </si>
 </sst>
 </file>
@@ -492,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,12 +1077,24 @@
       <c r="C41" s="3">
         <v>0.49305555555555558</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="B42" s="2">
+        <v>44865</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D42" s="1"/>
+      <c r="E42" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>

</xml_diff>

<commit_message>
changes made after call with Jan
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7830F22F-653E-468A-A38B-E34FD6CFED59}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08F70484-5073-4674-8069-0C30C95A563A}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,7 +166,7 @@
     <t>worked on pcb trace thickness</t>
   </si>
   <si>
-    <t>worked on PPT presentation for Thursday and enlarged pcb traces (for power)</t>
+    <t>worked on PPT presentation for Thursday and enlarged pcb traces (for power). Finished V0.1 of pcb (except for logo maybe)</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,14 +1091,20 @@
       <c r="C42" s="3">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="3">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E42" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="2">
+        <v>44866</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.375</v>
+      </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
return self state tryout excersise
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08F70484-5073-4674-8069-0C30C95A563A}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977AF9F4-2402-4D00-9180-5E1A782DF6E5}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Datum</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>worked on PPT presentation for Thursday and enlarged pcb traces (for power). Finished V0.1 of pcb (except for logo maybe)</t>
+  </si>
+  <si>
+    <t>Communicated with Jan on software, how to approach classes etc. Talked with jeroen -&gt; finished PCB order, PCB's are done for now. Went on a programming spree, wrote classes and unit tests</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1108,12 @@
       <c r="C43" s="3">
         <v>0.375</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>

</xml_diff>

<commit_message>
Tried to get pyqt working, and made template for testreport
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977AF9F4-2402-4D00-9180-5E1A782DF6E5}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACFE5861-51B6-489B-88D0-536F7D057E86}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Datum</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>Communicated with Jan on software, how to approach classes etc. Talked with jeroen -&gt; finished PCB order, PCB's are done for now. Went on a programming spree, wrote classes and unit tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created a lot of classes, rewrote classes, wrote unit tests, ended with steppermotor class. </t>
+  </si>
+  <si>
+    <t>Worked more on software, fixed motor class unit tests and held my mid term presentation</t>
+  </si>
+  <si>
+    <t>tried to get pyqt5 working in vsc (failed), finished creating test report templates</t>
   </si>
 </sst>
 </file>
@@ -501,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,19 +1125,46 @@
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="B44" s="2">
+        <v>44867</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="B45" s="2">
+        <v>44868</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="B46" s="2">
+        <v>44869</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>

</xml_diff>

<commit_message>
i2c esd circuit, log, picam2 main
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACFE5861-51B6-489B-88D0-536F7D057E86}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36372CEC-ED6F-43C0-A6E0-23720C3DD9D5}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Datum</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>tried to get pyqt5 working in vsc (failed), finished creating test report templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created test documents and did test for microscope led, made drawings. Fetched and created HCL boxes with components. Tried to fix pyqt5, again. </t>
+  </si>
+  <si>
+    <t>fixed bug that let pigpiod to not behave properly. Wrote testreport on stepper motor and got stepper motor working very well.</t>
   </si>
 </sst>
 </file>
@@ -243,6 +249,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,7 +521,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,19 +1177,43 @@
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="2">
+        <v>44872</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
+      <c r="B48" s="2">
+        <v>44873</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
+      <c r="B49" s="2">
+        <v>44874</v>
+      </c>
+      <c r="C49" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>

</xml_diff>

<commit_message>
add esd, log, extra order
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36372CEC-ED6F-43C0-A6E0-23720C3DD9D5}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AC80D3C-9A51-42EB-A078-491701D03B40}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Datum</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>fixed bug that let pigpiod to not behave properly. Wrote testreport on stepper motor and got stepper motor working very well.</t>
+  </si>
+  <si>
+    <t>ordered more parts, practiced soldering skills, talked with jelle about soldering approach and ordered more solder paste. Asked johan for components and paste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worked on raspberry pi camera implementation </t>
+  </si>
+  <si>
+    <t>working on raspberry pi camera.</t>
   </si>
 </sst>
 </file>
@@ -521,7 +530,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,7 +1213,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>44874</v>
       </c>
@@ -1214,78 +1223,97 @@
       <c r="D49" s="3">
         <v>0.70833333333333337</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="E49" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>44875</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>44879</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E51" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>

</xml_diff>

<commit_message>
updated main and log
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AC80D3C-9A51-42EB-A078-491701D03B40}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85BE0C3A-84FF-46B7-85B3-FA6FFF6BD718}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,7 +530,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1248,14 +1248,20 @@
       <c r="C51" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D51" s="1"/>
+      <c r="D51" s="3">
+        <v>0.625</v>
+      </c>
       <c r="E51" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="B52" s="2">
+        <v>44880</v>
+      </c>
+      <c r="C52" s="3">
+        <v>0.375</v>
+      </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
improvement list updated for pcb v0.2
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85BE0C3A-84FF-46B7-85B3-FA6FFF6BD718}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E3B9E44-46DA-4350-BDE0-6DC9EDCAB39F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Datum</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>working on raspberry pi camera.</t>
+  </si>
+  <si>
+    <t>pcb error debugging. Writing notes on v0.2</t>
+  </si>
+  <si>
+    <t>pdb error debugging, even more notes on v0.2</t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,12 +1268,26 @@
       <c r="C52" s="3">
         <v>0.375</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="B53" s="2">
+        <v>44881</v>
+      </c>
+      <c r="C53" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>

</xml_diff>

<commit_message>
started working on V1.4
-changed some footprints
-added/changed some LCSC values to/for components
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A38B42E5-5E57-45D9-8625-DA30FA690CC8}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30E11F54-B19D-4925-8F21-331934BC0F9D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>Datum</t>
   </si>
@@ -203,6 +203,18 @@
   </si>
   <si>
     <t>Even more pcb tests, debugging etc.</t>
+  </si>
+  <si>
+    <t>designed v0.2 of pcb</t>
+  </si>
+  <si>
+    <t>09:30?</t>
+  </si>
+  <si>
+    <t>finished designing v0.2 of pcb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attended UDC lessons and gave students feedback. Created pcb heater design and worked on camera. </t>
   </si>
 </sst>
 </file>
@@ -538,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1307,19 +1319,46 @@
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+      <c r="B55" s="2">
+        <v>44885</v>
+      </c>
+      <c r="C55" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+      <c r="B56" s="2">
+        <v>44886</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="B57" s="2">
+        <v>44887</v>
+      </c>
+      <c r="C57" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D57" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>

</xml_diff>

<commit_message>
improved LCSC + schematic values and order lists
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30E11F54-B19D-4925-8F21-331934BC0F9D}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
   <dimension ref="B1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Wrote documentation and finally got the multiple stepper drivers working on uart
</commit_message>
<xml_diff>
--- a/Documentation/LOG.xlsx
+++ b/Documentation/LOG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/jeroen_veen_han_nl/Documents/Research/Effluent/07 Studentprojects/Casper Tak/WaterQualityMonitor/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{739F6922-B31E-4F19-BEF9-4A0A40672144}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{A63433ED-A71D-4C96-BE8C-2E42C9D6FAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C126E09F-DA17-4FBD-8050-888F171BAC19}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Datum</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">worked on gui, guided s3 students, started test report on fluid movement. Worked on debugging stepper motor driver. Improved C++ programming and problem solving skills </t>
+  </si>
+  <si>
+    <t>Stopped logging</t>
   </si>
 </sst>
 </file>
@@ -291,10 +294,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -562,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
@@ -1443,10 +1442,10 @@
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="2">
-        <v>44895</v>
-      </c>
-      <c r="C63" s="1"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
@@ -1455,19 +1454,18 @@
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="1"/>
+      <c r="B65" s="2"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="1"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>

</xml_diff>